<commit_message>
refactor: Simplify Dosen management logic and enhance filtering capabilities
</commit_message>
<xml_diff>
--- a/public/sample/import-dosen.xlsx
+++ b/public/sample/import-dosen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B7BA71-CCD3-460C-92CA-DD59A5FE1D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08431692-C685-4F73-B0E2-F8FD45403FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5EACA6D-F844-44A0-AA30-A0DD1DB44018}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>NIP</t>
   </si>
@@ -42,41 +42,26 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
     <t>Aktif</t>
   </si>
   <si>
-    <t>Roles</t>
+    <t>sample123</t>
+  </si>
+  <si>
+    <t>Sample2</t>
   </si>
   <si>
     <t>Sample</t>
-  </si>
-  <si>
-    <t>Sample@gmail.com</t>
-  </si>
-  <si>
-    <t>sample123</t>
-  </si>
-  <si>
-    <t>dosen</t>
-  </si>
-  <si>
-    <t>Sample2</t>
-  </si>
-  <si>
-    <t>Sample2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,14 +77,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,7 +86,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,25 +109,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4502C1BB-781A-4A44-B06B-DC6A317B0E0F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,71 +470,52 @@
     <col min="6" max="6" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>123456789</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>987654321</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DCD6DB2E-CB14-4FCD-8D06-5ADD1E8E1E9F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F3CA0F2B-EC4B-4E50-8961-700AE50E2B3E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>